<commit_message>
22 53 Dec 29 2022
</commit_message>
<xml_diff>
--- a/src/test/resources/DefinitionData/DefinitionStorage_0.xlsx
+++ b/src/test/resources/DefinitionData/DefinitionStorage_0.xlsx
@@ -26,7 +26,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>D0.1596976872874879</t>
+    <t>D0.18565903795358007</t>
   </si>
   <si>
     <t>Automobile</t>
@@ -35,13 +35,13 @@
     <t>India</t>
   </si>
   <si>
-    <t>Sat, 10 Dec 2022 18:18:45 +0530</t>
+    <t>Mon, 19 Dec 2022 05:44:49 -0800</t>
   </si>
   <si>
-    <t>D0.7566317244104037</t>
+    <t>D0.3123609309210864</t>
   </si>
   <si>
-    <t>D0.5185698880184182</t>
+    <t>D0.6471154244116394</t>
   </si>
 </sst>
 </file>

</xml_diff>